<commit_message>
added wirefranes for bus hire site. Updated timeline. added cloud9 cheat sheet
</commit_message>
<xml_diff>
--- a/project_timeline.xlsx
+++ b/project_timeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Learn\CodeInstitute\DiplomainSoftwareDevelopment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8507BE-9D13-4D6D-9223-84594666D03B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA140EB-04F2-4224-9736-8FAAC4C387A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B4B30995-8F87-4E3B-B9C6-04CB76792ACA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="289">
   <si>
     <t>Completed</t>
   </si>
@@ -899,6 +899,9 @@
   </si>
   <si>
     <t>Actual</t>
+  </si>
+  <si>
+    <t>wireframe</t>
   </si>
 </sst>
 </file>
@@ -1365,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED276A9-7233-4140-A739-51159B902B77}">
   <dimension ref="A1:H511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="C97" workbookViewId="0">
+      <selection activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2099,6 +2102,9 @@
         <f t="shared" si="0"/>
         <v>44235</v>
       </c>
+      <c r="E57" s="9">
+        <v>44239</v>
+      </c>
     </row>
     <row r="58" spans="2:5">
       <c r="B58" s="4" t="s">
@@ -2123,6 +2129,9 @@
         <f t="shared" si="0"/>
         <v>44236</v>
       </c>
+      <c r="E59" s="9">
+        <v>44242</v>
+      </c>
     </row>
     <row r="60" spans="2:5">
       <c r="B60" s="3" t="s">
@@ -2135,6 +2144,9 @@
         <f t="shared" si="0"/>
         <v>44236</v>
       </c>
+      <c r="E60" s="9">
+        <v>44242</v>
+      </c>
     </row>
     <row r="61" spans="2:5">
       <c r="B61" s="3" t="s">
@@ -2147,6 +2159,9 @@
         <f t="shared" si="0"/>
         <v>44236</v>
       </c>
+      <c r="E61" s="9">
+        <v>44242</v>
+      </c>
     </row>
     <row r="62" spans="2:5">
       <c r="B62" s="3" t="s">
@@ -2158,6 +2173,9 @@
       <c r="D62" s="16">
         <f t="shared" si="0"/>
         <v>44236</v>
+      </c>
+      <c r="E62" s="9">
+        <v>44242</v>
       </c>
     </row>
     <row r="63" spans="2:5">
@@ -2519,7 +2537,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:8">
       <c r="B97" s="3" t="s">
         <v>99</v>
       </c>
@@ -2531,7 +2549,7 @@
         <v>44249</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:8">
       <c r="B98" s="3" t="s">
         <v>100</v>
       </c>
@@ -2543,7 +2561,7 @@
         <v>44249</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:8">
       <c r="B99" s="3" t="s">
         <v>101</v>
       </c>
@@ -2555,7 +2573,7 @@
         <v>44249</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:8">
       <c r="B100" s="3" t="s">
         <v>102</v>
       </c>
@@ -2567,14 +2585,14 @@
         <v>44249</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:8">
       <c r="B101" s="1"/>
       <c r="D101" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:8">
       <c r="B102" s="4" t="s">
         <v>70</v>
       </c>
@@ -2582,21 +2600,33 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F102" t="s">
+      <c r="F102" s="9">
+        <v>44238</v>
+      </c>
+      <c r="G102" t="s">
+        <v>288</v>
+      </c>
+      <c r="H102" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:8">
       <c r="B103" s="1"/>
       <c r="D103" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F103" t="s">
+      <c r="F103" s="9">
+        <v>44239</v>
+      </c>
+      <c r="G103" t="s">
+        <v>288</v>
+      </c>
+      <c r="H103" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:8">
       <c r="A104">
         <v>1</v>
       </c>
@@ -2610,11 +2640,11 @@
         <f t="shared" si="1"/>
         <v>44250</v>
       </c>
-      <c r="F104" t="s">
+      <c r="H104" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:8">
       <c r="A105">
         <v>2</v>
       </c>
@@ -2628,11 +2658,11 @@
         <f t="shared" si="1"/>
         <v>44251</v>
       </c>
-      <c r="F105" t="s">
+      <c r="H105" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="30">
+    <row r="106" spans="1:8" ht="30">
       <c r="A106">
         <v>3</v>
       </c>
@@ -2646,11 +2676,11 @@
         <f t="shared" si="1"/>
         <v>44252</v>
       </c>
-      <c r="F106" t="s">
+      <c r="H106" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:8">
       <c r="A107">
         <v>4</v>
       </c>
@@ -2667,11 +2697,11 @@
       <c r="E107" t="s">
         <v>261</v>
       </c>
-      <c r="F107" t="s">
+      <c r="H107" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:8">
       <c r="A108">
         <v>5</v>
       </c>
@@ -2685,11 +2715,11 @@
         <f t="shared" si="1"/>
         <v>44256</v>
       </c>
-      <c r="F108" t="s">
+      <c r="H108" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="14.25" customHeight="1">
+    <row r="109" spans="1:8" ht="14.25" customHeight="1">
       <c r="A109">
         <v>6</v>
       </c>
@@ -2703,11 +2733,11 @@
         <f t="shared" si="1"/>
         <v>44257</v>
       </c>
-      <c r="F109" t="s">
+      <c r="H109" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:8">
       <c r="A110">
         <v>7</v>
       </c>
@@ -2721,11 +2751,11 @@
         <f t="shared" si="1"/>
         <v>44258</v>
       </c>
-      <c r="F110" t="s">
+      <c r="H110" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="14.25" customHeight="1">
+    <row r="111" spans="1:8" ht="14.25" customHeight="1">
       <c r="A111">
         <v>8</v>
       </c>
@@ -2739,11 +2769,11 @@
         <f t="shared" si="1"/>
         <v>44259</v>
       </c>
-      <c r="F111" t="s">
+      <c r="H111" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:8">
       <c r="A112">
         <v>9</v>
       </c>
@@ -2757,7 +2787,7 @@
         <f t="shared" si="1"/>
         <v>44260</v>
       </c>
-      <c r="F112" t="s">
+      <c r="H112" t="s">
         <v>260</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added user stories. added responsive wireframe
</commit_message>
<xml_diff>
--- a/project_timeline.xlsx
+++ b/project_timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Learn\CodeInstitute\DiplomainSoftwareDevelopment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA140EB-04F2-4224-9736-8FAAC4C387A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9DE5E0-815A-4DDE-8DB0-62E8FC43048C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B4B30995-8F87-4E3B-B9C6-04CB76792ACA}"/>
   </bookViews>
@@ -1368,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED276A9-7233-4140-A739-51159B902B77}">
   <dimension ref="A1:H511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C97" workbookViewId="0">
-      <selection activeCell="F104" sqref="F104"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
updated timeline file with proress todate. just starting bootstrap.
</commit_message>
<xml_diff>
--- a/project_timeline.xlsx
+++ b/project_timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Learn\CodeInstitute\DiplomainSoftwareDevelopment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9DE5E0-815A-4DDE-8DB0-62E8FC43048C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DAA74E-792C-4720-8E1A-0D9B1ABF64F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B4B30995-8F87-4E3B-B9C6-04CB76792ACA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="290">
   <si>
     <t>Completed</t>
   </si>
@@ -902,6 +902,9 @@
   </si>
   <si>
     <t>wireframe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mentor Meeting MS1 One. Wireframes and user stories. </t>
   </si>
 </sst>
 </file>
@@ -1368,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED276A9-7233-4140-A739-51159B902B77}">
   <dimension ref="A1:H511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1996,7 +1999,7 @@
         <v>44232</v>
       </c>
     </row>
-    <row r="49" spans="2:5">
+    <row r="49" spans="2:6">
       <c r="B49" t="s">
         <v>268</v>
       </c>
@@ -2011,7 +2014,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="50" spans="2:5">
+    <row r="50" spans="2:6">
       <c r="B50" t="s">
         <v>268</v>
       </c>
@@ -2026,14 +2029,14 @@
         <v>268</v>
       </c>
     </row>
-    <row r="51" spans="2:5">
+    <row r="51" spans="2:6">
       <c r="B51" s="2"/>
       <c r="D51" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:5">
+    <row r="52" spans="2:6">
       <c r="B52" s="3" t="s">
         <v>71</v>
       </c>
@@ -2045,7 +2048,7 @@
         <v>44235</v>
       </c>
     </row>
-    <row r="53" spans="2:5">
+    <row r="53" spans="2:6">
       <c r="B53" s="1"/>
       <c r="C53" s="9">
         <v>44235</v>
@@ -2055,7 +2058,7 @@
         <v>44235</v>
       </c>
     </row>
-    <row r="54" spans="2:5">
+    <row r="54" spans="2:6">
       <c r="B54" s="4" t="s">
         <v>64</v>
       </c>
@@ -2067,7 +2070,7 @@
         <v>44235</v>
       </c>
     </row>
-    <row r="55" spans="2:5">
+    <row r="55" spans="2:6">
       <c r="B55" s="3" t="s">
         <v>72</v>
       </c>
@@ -2079,7 +2082,7 @@
         <v>44235</v>
       </c>
     </row>
-    <row r="56" spans="2:5">
+    <row r="56" spans="2:6">
       <c r="B56" s="3" t="s">
         <v>73</v>
       </c>
@@ -2091,7 +2094,7 @@
         <v>44235</v>
       </c>
     </row>
-    <row r="57" spans="2:5">
+    <row r="57" spans="2:6">
       <c r="B57" s="3" t="s">
         <v>74</v>
       </c>
@@ -2106,7 +2109,7 @@
         <v>44239</v>
       </c>
     </row>
-    <row r="58" spans="2:5">
+    <row r="58" spans="2:6">
       <c r="B58" s="4" t="s">
         <v>65</v>
       </c>
@@ -2118,7 +2121,7 @@
         <v>44236</v>
       </c>
     </row>
-    <row r="59" spans="2:5">
+    <row r="59" spans="2:6">
       <c r="B59" s="3" t="s">
         <v>75</v>
       </c>
@@ -2133,7 +2136,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="60" spans="2:5">
+    <row r="60" spans="2:6">
       <c r="B60" s="3" t="s">
         <v>76</v>
       </c>
@@ -2148,7 +2151,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="61" spans="2:5">
+    <row r="61" spans="2:6">
       <c r="B61" s="3" t="s">
         <v>77</v>
       </c>
@@ -2163,7 +2166,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="62" spans="2:5">
+    <row r="62" spans="2:6">
       <c r="B62" s="3" t="s">
         <v>78</v>
       </c>
@@ -2178,14 +2181,20 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="63" spans="2:5">
+    <row r="63" spans="2:6">
       <c r="B63" s="1"/>
       <c r="D63" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="2:5">
+      <c r="E63" s="9">
+        <v>44243</v>
+      </c>
+      <c r="F63" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6">
       <c r="B64" s="4" t="s">
         <v>66</v>
       </c>
@@ -2193,15 +2202,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="2:4">
+      <c r="E64" s="9">
+        <v>44243</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5">
       <c r="B65" s="1"/>
       <c r="D65" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="2:4">
+      <c r="E65" s="9">
+        <v>44243</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5">
       <c r="B66" s="3" t="s">
         <v>79</v>
       </c>
@@ -2212,8 +2227,11 @@
         <f t="shared" si="0"/>
         <v>44237</v>
       </c>
-    </row>
-    <row r="67" spans="2:4">
+      <c r="E66" s="9">
+        <v>44243</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5">
       <c r="B67" s="3" t="s">
         <v>80</v>
       </c>
@@ -2224,15 +2242,21 @@
         <f t="shared" ref="D67:D140" si="1">C67</f>
         <v>44237</v>
       </c>
-    </row>
-    <row r="68" spans="2:4">
+      <c r="E67" s="9">
+        <v>44243</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5">
       <c r="B68" s="1"/>
       <c r="D68" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="2:4">
+      <c r="E68" s="9">
+        <v>44243</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5">
       <c r="B69" s="4" t="s">
         <v>67</v>
       </c>
@@ -2240,15 +2264,21 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="2:4">
+      <c r="E69" s="9">
+        <v>44243</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5">
       <c r="B70" s="1"/>
       <c r="D70" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="2:4">
+      <c r="E70" s="9">
+        <v>44243</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5">
       <c r="B71" s="3" t="s">
         <v>81</v>
       </c>
@@ -2259,8 +2289,11 @@
         <f t="shared" si="1"/>
         <v>44238</v>
       </c>
-    </row>
-    <row r="72" spans="2:4">
+      <c r="E71" s="9">
+        <v>44243</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5">
       <c r="B72" s="3" t="s">
         <v>82</v>
       </c>
@@ -2271,8 +2304,11 @@
         <f t="shared" si="1"/>
         <v>44238</v>
       </c>
-    </row>
-    <row r="73" spans="2:4">
+      <c r="E72" s="9">
+        <v>44243</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5">
       <c r="B73" s="3" t="s">
         <v>83</v>
       </c>
@@ -2284,7 +2320,7 @@
         <v>44239</v>
       </c>
     </row>
-    <row r="74" spans="2:4">
+    <row r="74" spans="2:5">
       <c r="B74" s="3" t="s">
         <v>84</v>
       </c>
@@ -2296,7 +2332,7 @@
         <v>44240</v>
       </c>
     </row>
-    <row r="75" spans="2:4">
+    <row r="75" spans="2:5">
       <c r="B75" s="3" t="s">
         <v>85</v>
       </c>
@@ -2308,14 +2344,14 @@
         <v>44240</v>
       </c>
     </row>
-    <row r="76" spans="2:4">
+    <row r="76" spans="2:5">
       <c r="B76" s="1"/>
       <c r="D76" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:4">
+    <row r="77" spans="2:5">
       <c r="B77" s="4" t="s">
         <v>68</v>
       </c>
@@ -2324,14 +2360,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:4">
+    <row r="78" spans="2:5">
       <c r="B78" s="1"/>
       <c r="D78" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:4">
+    <row r="79" spans="2:5">
       <c r="B79" s="3" t="s">
         <v>86</v>
       </c>
@@ -2343,7 +2379,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="80" spans="2:4">
+    <row r="80" spans="2:5">
       <c r="B80" s="3" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
add bushire BOOTSTRAP site
</commit_message>
<xml_diff>
--- a/project_timeline.xlsx
+++ b/project_timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Learn\CodeInstitute\DiplomainSoftwareDevelopment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DAA74E-792C-4720-8E1A-0D9B1ABF64F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CB7DF8-8471-4A16-A0E0-7BCCF739EDEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B4B30995-8F87-4E3B-B9C6-04CB76792ACA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="291">
   <si>
     <t>Completed</t>
   </si>
@@ -905,6 +905,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mentor Meeting MS1 One. Wireframes and user stories. </t>
+  </si>
+  <si>
+    <t>Mentor Introduction.</t>
   </si>
 </sst>
 </file>
@@ -1371,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED276A9-7233-4140-A739-51159B902B77}">
   <dimension ref="A1:H511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1576,7 +1579,7 @@
         <v>Completed</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:6">
       <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
@@ -1588,7 +1591,7 @@
         <v>Completed</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:6">
       <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
@@ -1600,7 +1603,7 @@
         <v>Completed</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:6">
       <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
@@ -1612,7 +1615,7 @@
         <v>Completed</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:6">
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1624,7 +1627,7 @@
         <v>Completed</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:6">
       <c r="B21" s="3" t="s">
         <v>8</v>
       </c>
@@ -1638,8 +1641,11 @@
       <c r="E21" s="9">
         <v>44222</v>
       </c>
-    </row>
-    <row r="22" spans="2:5">
+      <c r="F21" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
       <c r="B22" s="3" t="s">
         <v>9</v>
       </c>
@@ -1654,7 +1660,7 @@
         <v>44222</v>
       </c>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:6">
       <c r="B23" s="3" t="s">
         <v>10</v>
       </c>
@@ -1669,7 +1675,7 @@
         <v>44222</v>
       </c>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:6">
       <c r="B24" s="3" t="s">
         <v>11</v>
       </c>
@@ -1684,7 +1690,7 @@
         <v>44223</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:6">
       <c r="B25" s="3" t="s">
         <v>12</v>
       </c>
@@ -1699,7 +1705,7 @@
         <v>44223</v>
       </c>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:6">
       <c r="B26" s="3" t="s">
         <v>13</v>
       </c>
@@ -1714,7 +1720,7 @@
         <v>44223</v>
       </c>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:6">
       <c r="B27" s="3" t="s">
         <v>14</v>
       </c>
@@ -1729,7 +1735,7 @@
         <v>44224</v>
       </c>
     </row>
-    <row r="28" spans="2:5">
+    <row r="28" spans="2:6">
       <c r="B28" s="3" t="s">
         <v>15</v>
       </c>
@@ -1744,7 +1750,7 @@
         <v>44224</v>
       </c>
     </row>
-    <row r="29" spans="2:5">
+    <row r="29" spans="2:6">
       <c r="B29" s="3" t="s">
         <v>16</v>
       </c>
@@ -1756,7 +1762,7 @@
         <v>44225</v>
       </c>
     </row>
-    <row r="30" spans="2:5">
+    <row r="30" spans="2:6">
       <c r="B30" s="3" t="s">
         <v>17</v>
       </c>
@@ -1768,7 +1774,7 @@
         <v>44225</v>
       </c>
     </row>
-    <row r="31" spans="2:5">
+    <row r="31" spans="2:6">
       <c r="B31" s="3" t="s">
         <v>18</v>
       </c>
@@ -1783,7 +1789,7 @@
         <v>44228</v>
       </c>
     </row>
-    <row r="32" spans="2:5">
+    <row r="32" spans="2:6">
       <c r="B32" s="3" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
added careers webinar. added ms1 webinar notes. updates to timeline.
</commit_message>
<xml_diff>
--- a/project_timeline.xlsx
+++ b/project_timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Learn\CodeInstitute\DiplomainSoftwareDevelopment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CB7DF8-8471-4A16-A0E0-7BCCF739EDEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45709620-8FFE-4586-88F4-9EBC3C91E910}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B4B30995-8F87-4E3B-B9C6-04CB76792ACA}"/>
   </bookViews>
@@ -1374,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED276A9-7233-4140-A739-51159B902B77}">
   <dimension ref="A1:H511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="B62" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2325,6 +2325,9 @@
         <f t="shared" si="1"/>
         <v>44239</v>
       </c>
+      <c r="E73" s="9">
+        <v>44250</v>
+      </c>
     </row>
     <row r="74" spans="2:5">
       <c r="B74" s="3" t="s">
@@ -2337,6 +2340,9 @@
         <f t="shared" si="1"/>
         <v>44240</v>
       </c>
+      <c r="E74" s="9">
+        <v>44250</v>
+      </c>
     </row>
     <row r="75" spans="2:5">
       <c r="B75" s="3" t="s">
@@ -2348,6 +2354,9 @@
       <c r="D75" s="16">
         <f t="shared" si="1"/>
         <v>44240</v>
+      </c>
+      <c r="E75" s="9">
+        <v>44250</v>
       </c>
     </row>
     <row r="76" spans="2:5">
@@ -2356,6 +2365,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="E76" s="9">
+        <v>44251</v>
+      </c>
     </row>
     <row r="77" spans="2:5">
       <c r="B77" s="4" t="s">
@@ -2364,6 +2376,9 @@
       <c r="D77" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="E77" s="9">
+        <v>44251</v>
       </c>
     </row>
     <row r="78" spans="2:5">
@@ -2372,6 +2387,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="E78" s="9">
+        <v>44251</v>
+      </c>
     </row>
     <row r="79" spans="2:5">
       <c r="B79" s="3" t="s">
@@ -2384,6 +2402,9 @@
         <f t="shared" si="1"/>
         <v>44242</v>
       </c>
+      <c r="E79" s="9">
+        <v>44251</v>
+      </c>
     </row>
     <row r="80" spans="2:5">
       <c r="B80" s="3" t="s">
@@ -2396,6 +2417,9 @@
         <f t="shared" si="1"/>
         <v>44242</v>
       </c>
+      <c r="E80" s="9">
+        <v>44251</v>
+      </c>
     </row>
     <row r="81" spans="2:5">
       <c r="B81" s="3" t="s">
@@ -2407,6 +2431,9 @@
       <c r="D81" s="16">
         <f t="shared" si="1"/>
         <v>44242</v>
+      </c>
+      <c r="E81" s="9">
+        <v>44252</v>
       </c>
     </row>
     <row r="82" spans="2:5">

</xml_diff>